<commit_message>
Working assembled ipynb file 1-7 chapters.
</commit_message>
<xml_diff>
--- a/HeroesOfPymoli/4_Age_Demographics.xlsx
+++ b/HeroesOfPymoli/4_Age_Demographics.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -369,17 +369,27 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Age Group</t>
+          <t>Age Category</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Bin Count</t>
+          <t>Purchase Count</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Percentage of Players</t>
+          <t>Average Purchase Price</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Total Purchase Value</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Average Total Purchase per Person</t>
         </is>
       </c>
     </row>
@@ -390,11 +400,21 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2.95%</t>
+          <t>$3.35</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>$77.13</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>$0.13</t>
         </is>
       </c>
     </row>
@@ -405,11 +425,21 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>3.82%</t>
+          <t>$2.96</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>$82.78</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>$0.14</t>
         </is>
       </c>
     </row>
@@ -420,11 +450,21 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>107</v>
+        <v>136</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>18.58%</t>
+          <t>$3.04</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>$412.89</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>$0.72</t>
         </is>
       </c>
     </row>
@@ -435,11 +475,21 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>258</v>
+        <v>365</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>44.79%</t>
+          <t>$3.05</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>$1,114.06</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>$1.93</t>
         </is>
       </c>
     </row>
@@ -450,11 +500,21 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>13.37%</t>
+          <t>$2.90</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>$293.00</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>$0.51</t>
         </is>
       </c>
     </row>
@@ -465,11 +525,21 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>9.03%</t>
+          <t>$2.93</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>$214.00</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>$0.37</t>
         </is>
       </c>
     </row>
@@ -480,11 +550,21 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>5.38%</t>
+          <t>$3.60</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>$147.67</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>$0.26</t>
         </is>
       </c>
     </row>
@@ -495,11 +575,21 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2.08%</t>
+          <t>$2.94</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>$38.24</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>$0.07</t>
         </is>
       </c>
     </row>

</xml_diff>